<commit_message>
Update overviews output files.
</commit_message>
<xml_diff>
--- a/schedules/schedule_classrooms-grouped_overview.xlsx
+++ b/schedules/schedule_classrooms-grouped_overview.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR5"/>
+  <dimension ref="A1:AR6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,6 +780,32 @@
       <c r="H3" t="n">
         <v>2</v>
       </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>2</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>7</v>
+      </c>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="inlineStr">
         <is>
@@ -827,6 +853,32 @@
       </c>
       <c r="AI3" t="n">
         <v>2</v>
+      </c>
+      <c r="AK3" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AL3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>7</v>
       </c>
     </row>
     <row r="4">
@@ -878,8 +930,60 @@
       <c r="Z4" t="n">
         <v>2</v>
       </c>
+      <c r="AB4" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AC4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>7</v>
+      </c>
       <c r="S5" s="1" t="n"/>
       <c r="T5" s="1" t="inlineStr">
         <is>
@@ -903,6 +1007,34 @@
       </c>
       <c r="Z5" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="S6" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>5</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0</v>
+      </c>
+      <c r="X6" t="n">
+        <v>2</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -921,7 +1053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR18"/>
+  <dimension ref="A1:AR19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1224,6 +1356,32 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" t="n">
+        <v>17</v>
+      </c>
+      <c r="E3" t="n">
+        <v>19</v>
+      </c>
+      <c r="F3" t="n">
+        <v>20</v>
+      </c>
+      <c r="G3" t="n">
+        <v>16</v>
+      </c>
+      <c r="H3" t="n">
+        <v>92</v>
+      </c>
       <c r="J3" s="1" t="n"/>
       <c r="K3" s="1" t="inlineStr">
         <is>
@@ -1492,6 +1650,32 @@
       <c r="AI5" t="n">
         <v>6</v>
       </c>
+      <c r="AK5" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AL5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>20</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>17</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>19</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>16</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>92</v>
+      </c>
     </row>
     <row r="6">
       <c r="J6" s="1" t="n"/>
@@ -1666,6 +1850,32 @@
       <c r="Q8" t="n">
         <v>16</v>
       </c>
+      <c r="S8" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="T8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="U8" t="n">
+        <v>20</v>
+      </c>
+      <c r="V8" t="n">
+        <v>17</v>
+      </c>
+      <c r="W8" t="n">
+        <v>19</v>
+      </c>
+      <c r="X8" t="n">
+        <v>20</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>92</v>
+      </c>
       <c r="AB8" s="1" t="n"/>
       <c r="AC8" s="1" t="inlineStr">
         <is>
@@ -1742,6 +1952,32 @@
       </c>
     </row>
     <row r="10">
+      <c r="J10" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="K10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="L10" t="n">
+        <v>20</v>
+      </c>
+      <c r="M10" t="n">
+        <v>17</v>
+      </c>
+      <c r="N10" t="n">
+        <v>19</v>
+      </c>
+      <c r="O10" t="n">
+        <v>20</v>
+      </c>
+      <c r="P10" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>92</v>
+      </c>
       <c r="AB10" s="1" t="n"/>
       <c r="AC10" s="1" t="inlineStr">
         <is>
@@ -1973,6 +2209,34 @@
       </c>
       <c r="AI18" t="n">
         <v>8</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="AB19" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AC19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>20</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>17</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>19</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>20</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>16</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1992,7 +2256,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR3"/>
+  <dimension ref="A1:AR4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2319,6 +2583,32 @@
       <c r="H3" t="n">
         <v>7</v>
       </c>
+      <c r="J3" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="K3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" t="n">
+        <v>3</v>
+      </c>
+      <c r="M3" t="n">
+        <v>3</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0</v>
+      </c>
+      <c r="P3" t="n">
+        <v>6</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>12</v>
+      </c>
       <c r="S3" s="1" t="n"/>
       <c r="T3" s="1" t="inlineStr">
         <is>
@@ -2390,6 +2680,112 @@
       </c>
       <c r="AR3" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>6</v>
+      </c>
+      <c r="H4" t="n">
+        <v>12</v>
+      </c>
+      <c r="S4" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="T4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3</v>
+      </c>
+      <c r="V4" t="n">
+        <v>3</v>
+      </c>
+      <c r="W4" t="n">
+        <v>0</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AB4" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AC4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AK4" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AL4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>6</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2409,7 +2805,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR21"/>
+  <dimension ref="A1:AR22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3296,6 +3692,32 @@
       <c r="AI7" t="n">
         <v>1</v>
       </c>
+      <c r="AK7" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AL7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>26</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>36</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>36</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>28</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>20</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n"/>
@@ -3322,6 +3744,32 @@
       <c r="H8" t="n">
         <v>2</v>
       </c>
+      <c r="J8" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="L8" t="n">
+        <v>26</v>
+      </c>
+      <c r="M8" t="n">
+        <v>36</v>
+      </c>
+      <c r="N8" t="n">
+        <v>36</v>
+      </c>
+      <c r="O8" t="n">
+        <v>28</v>
+      </c>
+      <c r="P8" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>146</v>
+      </c>
       <c r="S8" s="1" t="n"/>
       <c r="T8" s="1" t="inlineStr">
         <is>
@@ -3618,6 +4066,32 @@
       <c r="H12" t="n">
         <v>14</v>
       </c>
+      <c r="S12" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="T12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="U12" t="n">
+        <v>26</v>
+      </c>
+      <c r="V12" t="n">
+        <v>36</v>
+      </c>
+      <c r="W12" t="n">
+        <v>36</v>
+      </c>
+      <c r="X12" t="n">
+        <v>28</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>20</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>146</v>
+      </c>
       <c r="AB12" s="1" t="n"/>
       <c r="AC12" s="1" t="inlineStr">
         <is>
@@ -3718,6 +4192,32 @@
       <c r="H14" t="n">
         <v>8</v>
       </c>
+      <c r="AB14" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AC14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>26</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>36</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>36</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>28</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>146</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n"/>
@@ -3899,6 +4399,34 @@
       </c>
       <c r="H21" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="B22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="C22" t="n">
+        <v>26</v>
+      </c>
+      <c r="D22" t="n">
+        <v>36</v>
+      </c>
+      <c r="E22" t="n">
+        <v>36</v>
+      </c>
+      <c r="F22" t="n">
+        <v>28</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20</v>
+      </c>
+      <c r="H22" t="n">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -3919,7 +4447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR23"/>
+  <dimension ref="A1:AR24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4612,6 +5140,32 @@
       <c r="H6" t="n">
         <v>1</v>
       </c>
+      <c r="J6" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="L6" t="n">
+        <v>21</v>
+      </c>
+      <c r="M6" t="n">
+        <v>22</v>
+      </c>
+      <c r="N6" t="n">
+        <v>28</v>
+      </c>
+      <c r="O6" t="n">
+        <v>25</v>
+      </c>
+      <c r="P6" t="n">
+        <v>25</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>121</v>
+      </c>
       <c r="S6" s="1" t="n"/>
       <c r="T6" s="1" t="inlineStr">
         <is>
@@ -4659,6 +5213,32 @@
       </c>
       <c r="AI6" t="n">
         <v>5</v>
+      </c>
+      <c r="AK6" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AL6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>21</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>22</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>28</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>121</v>
       </c>
     </row>
     <row r="7">
@@ -5917,6 +6497,86 @@
       </c>
       <c r="AI23" t="n">
         <v>15</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="B24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="C24" t="n">
+        <v>21</v>
+      </c>
+      <c r="D24" t="n">
+        <v>22</v>
+      </c>
+      <c r="E24" t="n">
+        <v>28</v>
+      </c>
+      <c r="F24" t="n">
+        <v>25</v>
+      </c>
+      <c r="G24" t="n">
+        <v>25</v>
+      </c>
+      <c r="H24" t="n">
+        <v>121</v>
+      </c>
+      <c r="S24" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="T24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="U24" t="n">
+        <v>21</v>
+      </c>
+      <c r="V24" t="n">
+        <v>22</v>
+      </c>
+      <c r="W24" t="n">
+        <v>28</v>
+      </c>
+      <c r="X24" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>121</v>
+      </c>
+      <c r="AB24" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AC24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>22</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>28</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>25</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -5937,7 +6597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR10"/>
+  <dimension ref="A1:AR11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6386,6 +7046,32 @@
       <c r="H4" t="n">
         <v>5</v>
       </c>
+      <c r="J4" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="K4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="L4" t="n">
+        <v>7</v>
+      </c>
+      <c r="M4" t="n">
+        <v>4</v>
+      </c>
+      <c r="N4" t="n">
+        <v>7</v>
+      </c>
+      <c r="O4" t="n">
+        <v>8</v>
+      </c>
+      <c r="P4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>31</v>
+      </c>
       <c r="S4" s="1" t="n"/>
       <c r="T4" s="1" t="inlineStr">
         <is>
@@ -6433,6 +7119,32 @@
       </c>
       <c r="AI4" t="n">
         <v>6</v>
+      </c>
+      <c r="AK4" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AL4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>31</v>
       </c>
     </row>
     <row r="5">
@@ -6732,6 +7444,58 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F9" t="n">
+        <v>8</v>
+      </c>
+      <c r="G9" t="n">
+        <v>5</v>
+      </c>
+      <c r="H9" t="n">
+        <v>31</v>
+      </c>
+      <c r="S9" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="T9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="U9" t="n">
+        <v>7</v>
+      </c>
+      <c r="V9" t="n">
+        <v>4</v>
+      </c>
+      <c r="W9" t="n">
+        <v>7</v>
+      </c>
+      <c r="X9" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>31</v>
+      </c>
       <c r="AB9" s="1" t="n"/>
       <c r="AC9" s="1" t="inlineStr">
         <is>
@@ -6781,6 +7545,34 @@
       </c>
       <c r="AI10" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="AB11" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AC11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH11" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI11" t="n">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -6801,7 +7593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR41"/>
+  <dimension ref="A1:AR42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8176,6 +8968,32 @@
       <c r="AI11" t="n">
         <v>13</v>
       </c>
+      <c r="AK11" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AL11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>53</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>56</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>59</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>63</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>51</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>282</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -8398,6 +9216,32 @@
       <c r="H14" t="n">
         <v>7</v>
       </c>
+      <c r="J14" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="K14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="L14" t="n">
+        <v>53</v>
+      </c>
+      <c r="M14" t="n">
+        <v>56</v>
+      </c>
+      <c r="N14" t="n">
+        <v>59</v>
+      </c>
+      <c r="O14" t="n">
+        <v>63</v>
+      </c>
+      <c r="P14" t="n">
+        <v>51</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>282</v>
+      </c>
       <c r="S14" s="1" t="n"/>
       <c r="T14" s="1" t="inlineStr">
         <is>
@@ -9088,6 +9932,32 @@
       <c r="Z23" t="n">
         <v>11</v>
       </c>
+      <c r="AB23" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AC23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>53</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>56</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>59</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>63</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>51</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>282</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
@@ -9564,6 +10434,32 @@
       <c r="H33" t="n">
         <v>3</v>
       </c>
+      <c r="S33" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="T33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="U33" t="n">
+        <v>53</v>
+      </c>
+      <c r="V33" t="n">
+        <v>56</v>
+      </c>
+      <c r="W33" t="n">
+        <v>59</v>
+      </c>
+      <c r="X33" t="n">
+        <v>63</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>51</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>282</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n"/>
@@ -9771,6 +10667,34 @@
       </c>
       <c r="H41" t="n">
         <v>6</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="C42" t="n">
+        <v>53</v>
+      </c>
+      <c r="D42" t="n">
+        <v>56</v>
+      </c>
+      <c r="E42" t="n">
+        <v>59</v>
+      </c>
+      <c r="F42" t="n">
+        <v>63</v>
+      </c>
+      <c r="G42" t="n">
+        <v>51</v>
+      </c>
+      <c r="H42" t="n">
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -9791,7 +10715,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR33"/>
+  <dimension ref="A1:AR34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10922,6 +11846,32 @@
       <c r="AI9" t="n">
         <v>11</v>
       </c>
+      <c r="AK9" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AL9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>41</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>38</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>34</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>46</v>
+      </c>
+      <c r="AQ9" t="n">
+        <v>42</v>
+      </c>
+      <c r="AR9" t="n">
+        <v>201</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n"/>
@@ -11046,6 +11996,32 @@
       <c r="H11" t="n">
         <v>2</v>
       </c>
+      <c r="J11" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="K11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="L11" t="n">
+        <v>41</v>
+      </c>
+      <c r="M11" t="n">
+        <v>38</v>
+      </c>
+      <c r="N11" t="n">
+        <v>34</v>
+      </c>
+      <c r="O11" t="n">
+        <v>46</v>
+      </c>
+      <c r="P11" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>201</v>
+      </c>
       <c r="S11" s="1" t="n"/>
       <c r="T11" s="1" t="inlineStr">
         <is>
@@ -11416,6 +12392,32 @@
       <c r="H16" t="n">
         <v>2</v>
       </c>
+      <c r="S16" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="T16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="U16" t="n">
+        <v>41</v>
+      </c>
+      <c r="V16" t="n">
+        <v>38</v>
+      </c>
+      <c r="W16" t="n">
+        <v>34</v>
+      </c>
+      <c r="X16" t="n">
+        <v>46</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>42</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>201</v>
+      </c>
       <c r="AB16" s="1" t="n"/>
       <c r="AC16" s="1" t="inlineStr">
         <is>
@@ -11766,6 +12768,32 @@
       <c r="H23" t="n">
         <v>2</v>
       </c>
+      <c r="AB23" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="AC23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>41</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>38</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>34</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>46</v>
+      </c>
+      <c r="AH23" t="n">
+        <v>42</v>
+      </c>
+      <c r="AI23" t="n">
+        <v>201</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n"/>
@@ -12025,6 +13053,34 @@
       </c>
       <c r="H33" t="n">
         <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>Razem</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="C34" t="n">
+        <v>41</v>
+      </c>
+      <c r="D34" t="n">
+        <v>38</v>
+      </c>
+      <c r="E34" t="n">
+        <v>34</v>
+      </c>
+      <c r="F34" t="n">
+        <v>46</v>
+      </c>
+      <c r="G34" t="n">
+        <v>42</v>
+      </c>
+      <c r="H34" t="n">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>